<commit_message>
Feat : ExecCalcCombat 추가
</commit_message>
<xml_diff>
--- a/DesignData/Excel_Masters/WeaponStats_Master.xlsx
+++ b/DesignData/Excel_Masters/WeaponStats_Master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnrealCpp\Paradise\DesignData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnrealCpp\Paradise\DesignData\Excel_Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,10 +47,6 @@
     <t>SetID</t>
   </si>
   <si>
-    <t>Range</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Item.Type.Weapon.Melee.Sword</t>
   </si>
   <si>
@@ -122,6 +118,10 @@
   </si>
   <si>
     <t>Iron_Sword</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackRange</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1063,13 +1063,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1078,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -1096,15 +1096,15 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1125,13 +1125,13 @@
         <v>0.2</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1206,27 +1206,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1247,27 +1247,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>